<commit_message>
Adding the change passowrd option to the admin and unite the select role of the user in the creation process
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,7 +500,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -514,7 +510,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>00:15 19/12/2025</t>
+          <t>23:24 28/12/2025</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -531,7 +527,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>M1</t>
+          <t>M</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -545,18 +541,15 @@
       <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3" t="b">
         <v>0</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="2" t="n">
-        <v>46008.88019956018</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>user_photo.png</t>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>23:45 28/12/2025</t>
         </is>
       </c>
     </row>
@@ -580,20 +573,51 @@
         </is>
       </c>
       <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>23:45 28/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>איתי</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>2</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F5" t="b">
         <v>0</v>
       </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>46008.88019956018</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>user_photo.png</t>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>23:46 28/12/2025</t>
         </is>
       </c>
     </row>

</xml_diff>